<commit_message>
Update Gantt Chart for Echolocation V2.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Gantt Chart for Echolocation V2.xlsx
+++ b/Documents/Gantt Chart for Echolocation V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai Kothari\Documents\Uni\First Year\Term 2\Game Prototype Development - IMAT1910\Coursework\Final\Echolocation\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{303B90FD-7738-4BA0-B9A8-9475AEFE41A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A230E0-C0C7-4A46-8F0E-4F2FC699DACF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -238,9 +238,6 @@
     <t>PERIODS - IN DAYS - START DATE: 23/02/2020 - END DATE: 18/04/2020 - TOTAL DAYS: 55 DAYS</t>
   </si>
   <si>
-    <t>A Gantt Chart showing the development of  the game Echolocation for IMAT1910 - Game Prototype Development</t>
-  </si>
-  <si>
     <t>Scripts - Sound Manager</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>Scripts - Water</t>
+  </si>
+  <si>
+    <t>A Gantt Chart showing the development of the game Echolocation for IMAT1910 - Game Prototype Development</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1070,8 @@
   </sheetPr>
   <dimension ref="B1:BJ38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="2" spans="2:62" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="24" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="15" spans="2:62" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="7">
         <v>21</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="7">
         <v>21</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="7">
         <v>35</v>

</xml_diff>